<commit_message>
added test case for AutoMOF_6 series
</commit_message>
<xml_diff>
--- a/tests/testData/AutoMOFs05_Solution0.xlsx
+++ b/tests/testData/AutoMOFs05_Solution0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Code\DACHS\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Code\DACHS\tests\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D260046E-BD9B-47A0-8D4C-888BD1E7DA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6DC14F4-3A34-4A64-9F3D-8B3CFBBAF2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16296" yWindow="3852" windowWidth="30960" windowHeight="12204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,22 +79,22 @@
     <t>29.5631</t>
   </si>
   <si>
-    <t xml:space="preserve"> Zn6H002</t>
-  </si>
-  <si>
     <t>477.6</t>
   </si>
   <si>
-    <t xml:space="preserve"> MeOH002</t>
-  </si>
-  <si>
     <t xml:space="preserve"> g</t>
   </si>
   <si>
-    <t xml:space="preserve"> Weight MeOH_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Weight Zn6H_2</t>
+    <t xml:space="preserve"> Zn6H_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MeOH_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mass of Zn6H_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> mass of MeOH_2</t>
   </si>
 </sst>
 </file>
@@ -499,19 +499,19 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.20703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.1015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -557,7 +557,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -571,16 +571,16 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -597,13 +597,13 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -617,16 +617,16 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" t="s">
         <v>20</v>
       </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -643,13 +643,13 @@
         <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>10</v>
       </c>

</xml_diff>